<commit_message>
Something with my implementation of the upsampling layers in a network is messed up. Why?
</commit_message>
<xml_diff>
--- a/Documents/FeatureMapCalculator.xlsx
+++ b/Documents/FeatureMapCalculator.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lamcnguyen/Softwaredev/CAP5415_Assignments/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C31227D-AF47-5747-AC54-AD0AA17E5EA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{272CBBFE-FE3E-AE4F-AB95-9A1ACC950BD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2180" yWindow="4320" windowWidth="16040" windowHeight="17440" xr2:uid="{AE9F49A2-4307-0D4C-984B-2F75C0F7ECE1}"/>
+    <workbookView xWindow="1520" yWindow="5920" windowWidth="18220" windowHeight="17440" xr2:uid="{AE9F49A2-4307-0D4C-984B-2F75C0F7ECE1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="14">
   <si>
     <t>Padding</t>
   </si>
@@ -74,6 +74,9 @@
   </si>
   <si>
     <t>Feature Map Edge Length Calculator 1D</t>
+  </si>
+  <si>
+    <t>output padding must be smaller then stride or dilation</t>
   </si>
 </sst>
 </file>
@@ -442,16 +445,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D100A23-660C-F641-83CF-D74D759B4151}">
-  <dimension ref="A1:H12"/>
+  <dimension ref="A1:H16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="16.6640625" customWidth="1"/>
-    <col min="2" max="2" width="21" customWidth="1"/>
+    <col min="2" max="2" width="21.83203125" customWidth="1"/>
     <col min="3" max="3" width="20" customWidth="1"/>
     <col min="8" max="8" width="15.5" customWidth="1"/>
   </cols>
@@ -530,7 +533,7 @@
         <v>5</v>
       </c>
       <c r="C4">
-        <f t="shared" ref="C4:C12" si="1">B3</f>
+        <f t="shared" ref="C4:C6" si="1">B3</f>
         <v>10</v>
       </c>
       <c r="D4">
@@ -555,7 +558,7 @@
       </c>
       <c r="B5">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C5">
         <f t="shared" si="1"/>
@@ -571,7 +574,7 @@
         <v>3</v>
       </c>
       <c r="G5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H5">
         <v>0</v>
@@ -583,11 +586,11 @@
       </c>
       <c r="B6">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C6">
         <f t="shared" si="1"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D6">
         <v>0</v>
@@ -607,141 +610,146 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B7">
-        <f>(C7-1)*E7-2*D7+G7*(F7-1)+H7+1</f>
-        <v>3</v>
+        <f>C7*2</f>
+        <v>2</v>
       </c>
       <c r="C7">
-        <f t="shared" si="1"/>
-        <v>2</v>
-      </c>
-      <c r="D7">
-        <v>1</v>
-      </c>
-      <c r="E7">
-        <v>2</v>
-      </c>
-      <c r="F7">
-        <v>3</v>
-      </c>
-      <c r="G7">
-        <v>1</v>
-      </c>
-      <c r="H7">
-        <v>0</v>
-      </c>
+        <f>B6</f>
+        <v>1</v>
+      </c>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B8">
-        <f>C8*2</f>
-        <v>6</v>
+        <f>(C8-1)*E8-2*D8+G8*(F8-1)+H8+1</f>
+        <v>2</v>
       </c>
       <c r="C8">
-        <f t="shared" si="1"/>
+        <f>B7</f>
+        <v>2</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+      <c r="F8">
         <v>3</v>
       </c>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
-      <c r="G8" s="1"/>
-      <c r="H8" s="1"/>
+      <c r="G8">
+        <v>1</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B9">
-        <f>(C9-1)*E9-2*D9+G9*(F9-1)+H9+1</f>
-        <v>6</v>
+        <f>C9*2</f>
+        <v>4</v>
       </c>
       <c r="C9">
-        <f t="shared" si="1"/>
-        <v>6</v>
-      </c>
-      <c r="D9">
-        <v>1</v>
-      </c>
-      <c r="E9">
-        <v>1</v>
-      </c>
-      <c r="F9">
-        <v>3</v>
-      </c>
-      <c r="G9">
-        <v>1</v>
-      </c>
-      <c r="H9">
-        <v>0</v>
-      </c>
+        <f>B8</f>
+        <v>2</v>
+      </c>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B10">
-        <f>C10*2</f>
-        <v>12</v>
+        <f>(C10-1)*E10-2*D10+G10*(F10-1)+H10+1</f>
+        <v>7</v>
       </c>
       <c r="C10">
-        <f t="shared" si="1"/>
-        <v>6</v>
-      </c>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
-      <c r="H10" s="1"/>
+        <f>B9</f>
+        <v>4</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="E10">
+        <v>2</v>
+      </c>
+      <c r="F10">
+        <v>3</v>
+      </c>
+      <c r="G10">
+        <v>1</v>
+      </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11">
+        <f>C11*2</f>
+        <v>14</v>
+      </c>
+      <c r="C11">
+        <f>B10</f>
         <v>7</v>
       </c>
-      <c r="B11">
-        <f>(C11-1)*E11-2*D11+G11*(F11-1)+H11+1</f>
-        <v>14</v>
-      </c>
-      <c r="C11">
-        <f t="shared" si="1"/>
-        <v>12</v>
-      </c>
-      <c r="D11">
-        <v>1</v>
-      </c>
-      <c r="E11">
-        <v>1</v>
-      </c>
-      <c r="F11">
-        <v>3</v>
-      </c>
-      <c r="G11">
-        <v>2</v>
-      </c>
-      <c r="H11">
-        <v>0</v>
-      </c>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B12">
-        <f>C12*2</f>
+        <f>(C12-1)*E12-2*D12+G12*(F12-1)+H12+1</f>
         <v>28</v>
       </c>
       <c r="C12">
-        <f t="shared" si="1"/>
+        <f>B11</f>
         <v>14</v>
       </c>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
-      <c r="G12" s="1"/>
-      <c r="H12" s="1"/>
+      <c r="D12">
+        <v>1</v>
+      </c>
+      <c r="E12">
+        <v>2</v>
+      </c>
+      <c r="F12">
+        <v>3</v>
+      </c>
+      <c r="G12">
+        <v>1</v>
+      </c>
+      <c r="H12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F16" t="s">
+        <v>13</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Slowly improving the CNN model but still not sure why the output image is the wrong sized tensor
</commit_message>
<xml_diff>
--- a/Documents/FeatureMapCalculator.xlsx
+++ b/Documents/FeatureMapCalculator.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lamcnguyen/Softwaredev/CAP5415_Assignments/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{272CBBFE-FE3E-AE4F-AB95-9A1ACC950BD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5D192F5-1C8A-D042-BF7C-D310E646C91E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1520" yWindow="5920" windowWidth="18220" windowHeight="17440" xr2:uid="{AE9F49A2-4307-0D4C-984B-2F75C0F7ECE1}"/>
+    <workbookView xWindow="0" yWindow="8740" windowWidth="17240" windowHeight="13900" xr2:uid="{AE9F49A2-4307-0D4C-984B-2F75C0F7ECE1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="14">
   <si>
     <t>Padding</t>
   </si>
@@ -445,10 +445,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D100A23-660C-F641-83CF-D74D759B4151}">
-  <dimension ref="A1:H16"/>
+  <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -558,7 +558,7 @@
       </c>
       <c r="B5">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C5">
         <f t="shared" si="1"/>
@@ -574,7 +574,7 @@
         <v>3</v>
       </c>
       <c r="G5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H5">
         <v>0</v>
@@ -586,11 +586,11 @@
       </c>
       <c r="B6">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C6">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D6">
         <v>0</v>
@@ -610,21 +610,31 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B7">
-        <f>C7*2</f>
-        <v>2</v>
+        <f>(C7-1)*E7-2*D7+G7*(F7-1)+H7+1</f>
+        <v>3</v>
       </c>
       <c r="C7">
         <f>B6</f>
-        <v>1</v>
-      </c>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
-      <c r="H7" s="1"/>
+        <v>2</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7">
+        <v>2</v>
+      </c>
+      <c r="F7">
+        <v>3</v>
+      </c>
+      <c r="G7">
+        <v>1</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
@@ -632,17 +642,17 @@
       </c>
       <c r="B8">
         <f>(C8-1)*E8-2*D8+G8*(F8-1)+H8+1</f>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C8">
         <f>B7</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D8">
         <v>1</v>
       </c>
       <c r="E8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F8">
         <v>3</v>
@@ -660,11 +670,11 @@
       </c>
       <c r="B9">
         <f>C9*2</f>
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="C9">
         <f>B8</f>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
@@ -678,17 +688,17 @@
       </c>
       <c r="B10">
         <f>(C10-1)*E10-2*D10+G10*(F10-1)+H10+1</f>
-        <v>7</v>
+        <v>28</v>
       </c>
       <c r="C10">
         <f>B9</f>
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="D10">
         <v>1</v>
       </c>
       <c r="E10">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F10">
         <v>3</v>
@@ -700,54 +710,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A11" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B11">
-        <f>C11*2</f>
-        <v>14</v>
-      </c>
-      <c r="C11">
-        <f>B10</f>
-        <v>7</v>
-      </c>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
-      <c r="G11" s="1"/>
-      <c r="H11" s="1"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A12" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B12">
-        <f>(C12-1)*E12-2*D12+G12*(F12-1)+H12+1</f>
-        <v>28</v>
-      </c>
-      <c r="C12">
-        <f>B11</f>
-        <v>14</v>
-      </c>
-      <c r="D12">
-        <v>1</v>
-      </c>
-      <c r="E12">
-        <v>2</v>
-      </c>
-      <c r="F12">
-        <v>3</v>
-      </c>
-      <c r="G12">
-        <v>1</v>
-      </c>
-      <c r="H12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="F16" t="s">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F14" t="s">
         <v>13</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added links for Course Project
</commit_message>
<xml_diff>
--- a/Documents/FeatureMapCalculator.xlsx
+++ b/Documents/FeatureMapCalculator.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="14">
   <si>
     <t xml:space="preserve">Feature Map Edge Length Calculator 1D</t>
   </si>
@@ -188,10 +188,10 @@
   <dimension ref="A1:H24"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F24" activeCellId="0" sqref="F24"/>
+      <selection pane="topLeft" activeCell="F19" activeCellId="0" sqref="F19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.50390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="21.83"/>
@@ -468,7 +468,7 @@
       </c>
       <c r="B19" s="0" t="n">
         <f aca="false">((C19+2*D19-G19*(F19-1)-1)/E19)+1</f>
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C19" s="0" t="n">
         <v>32</v>
@@ -480,7 +480,7 @@
         <v>1</v>
       </c>
       <c r="F19" s="0" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="G19" s="0" t="n">
         <v>1</v>
@@ -495,11 +495,11 @@
       </c>
       <c r="B20" s="0" t="n">
         <f aca="false">((C20+2*D20-G20*(F20-1)-1)/E20)+1</f>
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C20" s="0" t="n">
         <f aca="false">B19</f>
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D20" s="0" t="n">
         <v>0</v>
@@ -523,11 +523,11 @@
       </c>
       <c r="B21" s="0" t="n">
         <f aca="false">((C21+2*D21-G21*(F21-1)-1)/E21)+1</f>
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C21" s="0" t="n">
         <f aca="false">B20</f>
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D21" s="0" t="n">
         <v>0</v>
@@ -536,7 +536,7 @@
         <v>1</v>
       </c>
       <c r="F21" s="0" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="G21" s="0" t="n">
         <v>1</v>
@@ -551,11 +551,11 @@
       </c>
       <c r="B22" s="0" t="n">
         <f aca="false">((C22+2*D22-G22*(F22-1)-1)/E22)+1</f>
-        <v>6.5</v>
+        <v>5</v>
       </c>
       <c r="C22" s="0" t="n">
         <f aca="false">B21</f>
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="D22" s="0" t="n">
         <v>0</v>
@@ -579,11 +579,11 @@
       </c>
       <c r="B23" s="0" t="n">
         <f aca="false">((C23+2*D23-G23*(F23-1)-1)/E23)+1</f>
-        <v>4.5</v>
+        <v>4</v>
       </c>
       <c r="C23" s="0" t="n">
         <f aca="false">B22</f>
-        <v>6.5</v>
+        <v>5</v>
       </c>
       <c r="D23" s="0" t="n">
         <v>0</v>
@@ -592,7 +592,7 @@
         <v>1</v>
       </c>
       <c r="F23" s="0" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G23" s="0" t="n">
         <v>1</v>
@@ -602,6 +602,29 @@
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B24" s="0" t="n">
+        <f aca="false">((C24+2*D24-G24*(F24-1)-1)/E24)+1</f>
+        <v>3</v>
+      </c>
+      <c r="C24" s="0" t="n">
+        <f aca="false">B23</f>
+        <v>4</v>
+      </c>
+      <c r="D24" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E24" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F24" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="G24" s="0" t="n">
+        <v>1</v>
+      </c>
       <c r="H24" s="0" t="n">
         <v>0</v>
       </c>

</xml_diff>